<commit_message>
First db service (examplary) finished - login
</commit_message>
<xml_diff>
--- a/Dokumenti/DB services.xlsx
+++ b/Dokumenti/DB services.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="56">
   <si>
     <t>SERVISI ZA BAZU</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>Inactive</t>
+  </si>
+  <si>
+    <t>Ready</t>
   </si>
 </sst>
 </file>
@@ -571,17 +574,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperveza" xfId="1" builtinId="8"/>
@@ -894,10 +897,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,57 +913,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
       <c r="H1" s="21"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="F2" s="21"/>
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="23" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1001,7 +1004,7 @@
         <v>15</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Login service aktiviran, dignuto na server
</commit_message>
<xml_diff>
--- a/Dokumenti/DB services.xlsx
+++ b/Dokumenti/DB services.xlsx
@@ -79,9 +79,6 @@
     <t>ROOT:</t>
   </si>
   <si>
-    <t>http://vdl.hr/</t>
-  </si>
-  <si>
     <t>user/login</t>
   </si>
   <si>
@@ -220,14 +217,17 @@
     <t>Inactive</t>
   </si>
   <si>
-    <t>Ready</t>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>http://vdl.hr/ferbook/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,15 +302,6 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -575,7 +566,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -585,6 +575,7 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperveza" xfId="1" builtinId="8"/>
@@ -897,10 +888,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,58 +904,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
       <c r="H1" s="21"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="F2" s="21"/>
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="23" t="s">
-        <v>8</v>
+      <c r="B9" s="26" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -978,10 +969,10 @@
         <v>5</v>
       </c>
       <c r="D10" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="20" t="s">
         <v>12</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>13</v>
       </c>
       <c r="F10" s="19" t="s">
         <v>6</v>
@@ -989,322 +980,322 @@
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="C11" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>17</v>
-      </c>
       <c r="C12" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>21</v>
-      </c>
       <c r="E13" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="E14" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>25</v>
-      </c>
       <c r="E15" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="C17" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>31</v>
-      </c>
       <c r="E17" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="C18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>34</v>
-      </c>
       <c r="E18" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="C19" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>38</v>
-      </c>
       <c r="E20" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="195" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="195" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>42</v>
-      </c>
       <c r="C23" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>46</v>
-      </c>
       <c r="C24" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="C25" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="C26" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>53</v>
-      </c>
       <c r="E26" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Registracija dodana, popravljene sitnice oko logina
</commit_message>
<xml_diff>
--- a/Dokumenti/DB services.xlsx
+++ b/Dokumenti/DB services.xlsx
@@ -566,6 +566,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -575,7 +576,6 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperveza" xfId="1" builtinId="8"/>
@@ -888,10 +888,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,57 +904,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
       <c r="H1" s="21"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="F2" s="21"/>
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="23" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1035,7 +1035,7 @@
         <v>14</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Završeni svi message servisi ( inbox i send dodani)
</commit_message>
<xml_diff>
--- a/Dokumenti/DB services.xlsx
+++ b/Dokumenti/DB services.xlsx
@@ -163,9 +163,6 @@
     <t>messages/inbox</t>
   </si>
   <si>
-    <t>{ "data" : [{"userId": id, "name":name, "lastname":lastname, "email":email, "username":username, "lastMessage" : {"messageId":id, "message":message, "timestamp":timestamp, "flag":flag}}, {second conversation}, {third conversation}, …, {nth conversation}] , "error" : [] }</t>
-  </si>
-  <si>
     <t>post/newsfeed</t>
   </si>
   <si>
@@ -221,6 +218,9 @@
   </si>
   <si>
     <t>{ "data" : [ {"message" : message, "senderId": sender,  "timestamp" : timestamp, "flag": flag} , {second message}, {third message}, … {nth message}] , "error" : [] }</t>
+  </si>
+  <si>
+    <t>{ "data" : [{"userId": id, "name":name, "lastname":lastname, "lastMessage" : { "message":message, "senderId": sender, "timestamp":timestamp, "flag":flag}}, {second conversation}, {third conversation}, …, {nth conversation}] , "error" : [] }</t>
   </si>
 </sst>
 </file>
@@ -889,7 +889,7 @@
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -953,7 +953,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="21.75" thickBot="1">
@@ -993,7 +993,7 @@
         <v>14</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="45">
@@ -1013,7 +1013,7 @@
         <v>14</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30">
@@ -1033,7 +1033,7 @@
         <v>14</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30">
@@ -1053,7 +1053,7 @@
         <v>14</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30">
@@ -1073,7 +1073,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30">
@@ -1087,13 +1087,13 @@
         <v>10</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30">
@@ -1113,7 +1113,7 @@
         <v>14</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="60">
@@ -1127,13 +1127,13 @@
         <v>10</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30">
@@ -1156,7 +1156,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="105">
+    <row r="20" spans="1:6" ht="90">
       <c r="A20" s="11" t="s">
         <v>35</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>10</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>14</v>
@@ -1178,122 +1178,122 @@
     </row>
     <row r="21" spans="1:6" ht="195">
       <c r="A21" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="195">
       <c r="A22" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E22" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30">
       <c r="A23" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="C23" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30">
       <c r="A24" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>44</v>
-      </c>
       <c r="C24" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30">
       <c r="A25" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>48</v>
-      </c>
       <c r="C25" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="60.75" thickBot="1">
       <c r="A26" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="C26" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="17" t="s">
+      <c r="E26" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="18" t="s">
         <v>51</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
User/edit i user/info dodani
</commit_message>
<xml_diff>
--- a/Dokumenti/DB services.xlsx
+++ b/Dokumenti/DB services.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="20730" windowHeight="11760"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="58">
   <si>
     <t>SERVISI ZA BAZU</t>
   </si>
@@ -221,13 +221,19 @@
   </si>
   <si>
     <t>{ "data" : [{"userId": id, "name":name, "lastname":lastname, "lastMessage" : { "message":message, "senderId": sender, "timestamp":timestamp, "flag":flag}}, {second conversation}, {third conversation}, …, {nth conversation}] , "error" : [] }</t>
+  </si>
+  <si>
+    <t>{username, password, name, lastname }</t>
+  </si>
+  <si>
+    <t>Ready</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -578,8 +584,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hiperveza" xfId="1" builtinId="8"/>
+    <cellStyle name="Normalno" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -600,7 +606,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema sustava Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -674,6 +680,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -708,6 +715,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -883,16 +891,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
@@ -901,7 +909,7 @@
     <col min="5" max="5" width="70" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -913,7 +921,7 @@
       <c r="G1" s="21"/>
       <c r="H1" s="21"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -923,7 +931,7 @@
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
@@ -933,14 +941,14 @@
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>2</v>
       </c>
@@ -948,7 +956,7 @@
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1">
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>7</v>
       </c>
@@ -956,7 +964,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" ht="21.75" thickBot="1">
+    <row r="10" spans="1:8" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="19" t="s">
         <v>3</v>
       </c>
@@ -976,7 +984,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -996,7 +1004,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="45">
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>15</v>
       </c>
@@ -1013,10 +1021,10 @@
         <v>14</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -1036,12 +1044,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>10</v>
@@ -1053,10 +1061,10 @@
         <v>14</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="30">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>23</v>
       </c>
@@ -1076,7 +1084,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>25</v>
       </c>
@@ -1096,7 +1104,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>28</v>
       </c>
@@ -1116,7 +1124,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="60">
+    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>31</v>
       </c>
@@ -1136,7 +1144,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>33</v>
       </c>
@@ -1156,7 +1164,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="90">
+    <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>35</v>
       </c>
@@ -1176,7 +1184,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="195">
+    <row r="21" spans="1:6" ht="195" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>36</v>
       </c>
@@ -1196,7 +1204,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="195">
+    <row r="22" spans="1:6" ht="195" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>37</v>
       </c>
@@ -1216,7 +1224,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>38</v>
       </c>
@@ -1236,7 +1244,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="30">
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>42</v>
       </c>
@@ -1256,7 +1264,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="30">
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>46</v>
       </c>
@@ -1276,7 +1284,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="60.75" thickBot="1">
+    <row r="26" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>48</v>
       </c>
@@ -1317,24 +1325,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Post newsfeed, publish i comment dodani
</commit_message>
<xml_diff>
--- a/Dokumenti/DB services.xlsx
+++ b/Dokumenti/DB services.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="20100" windowHeight="7785"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
   <si>
     <t>SERVISI ZA BAZU</t>
   </si>
@@ -172,9 +172,6 @@
     <t>post/publish</t>
   </si>
   <si>
-    <t>{userId1, userId2, message, url}</t>
-  </si>
-  <si>
     <t>{ "data" : ["url":url] , "error" : [] }</t>
   </si>
   <si>
@@ -196,9 +193,6 @@
     <t>post/comment</t>
   </si>
   <si>
-    <t>{userId, postId, text}</t>
-  </si>
-  <si>
     <t>search</t>
   </si>
   <si>
@@ -226,7 +220,19 @@
     <t>{username, password, name, lastname }</t>
   </si>
   <si>
-    <t>Ready</t>
+    <t>{sender, recipient, message, url}</t>
+  </si>
+  <si>
+    <t>{userId, postId, message}</t>
+  </si>
+  <si>
+    <t>post/getComments</t>
+  </si>
+  <si>
+    <t>{ "data" : [{"postId":id, "text" : text, "url":"url", "timestamp" : timestamp,"userId":id, "name":name, "lastName":lastname, "profilePicture":url, "username":username}, {second comment}, …{nth comment}] , "error" : [] }</t>
+  </si>
+  <si>
+    <t>{ "data" : [postId : {"postId":id, "text" : text, "url":"url", "timestamp" : timestamp,"userId":id, "name":name, "lastName":lastname, "profilePicture":url, "username":username, "comments" : commentsNmbr, "likes": likesNmbr}, secondPost : {secondPost}, .. nthPost : {nthPost}] , "error" : [] }</t>
   </si>
 </sst>
 </file>
@@ -892,12 +898,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +967,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -1001,7 +1007,7 @@
         <v>14</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1021,7 +1027,7 @@
         <v>14</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1041,7 +1047,7 @@
         <v>14</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1049,7 +1055,7 @@
         <v>21</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>10</v>
@@ -1061,7 +1067,7 @@
         <v>14</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1081,7 +1087,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1095,13 +1101,13 @@
         <v>10</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1121,7 +1127,7 @@
         <v>14</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1135,13 +1141,13 @@
         <v>10</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1161,7 +1167,7 @@
         <v>14</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1175,133 +1181,153 @@
         <v>10</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="195" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B21" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="195" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="195" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="B26" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B27" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="15" t="s">
+      <c r="C27" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="E27" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="18" t="s">
         <v>49</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1310,7 +1336,7 @@
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A1:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="F11:F26">
+  <conditionalFormatting sqref="F11:F27">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Active"</formula>
     </cfRule>

</xml_diff>

<commit_message>
post/wall i post/getComments dodani i aktivni, promjene u excel fileu za pozivanje nad istima
</commit_message>
<xml_diff>
--- a/Dokumenti/DB services.xlsx
+++ b/Dokumenti/DB services.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="59">
   <si>
     <t>SERVISI ZA BAZU</t>
   </si>
@@ -184,9 +184,6 @@
     <t>{userId, postId, flag}</t>
   </si>
   <si>
-    <t>{ "data" : [{"postId":id, "text" : text, "url":"url", "timestamp" : timestamp,"userId":id, "name":name, "lastName":lastname, "profilePicture":url, "username":username, "comments" : [ {"commentId":id, "text":text, "timestamp":timestamp, "userId":id, "name":name, "lastName":lastaname, "profilePicture":url, "username":username}, {second comment}, {third comment}, …, {nth comment} ], "likes": [ {"userId":id, "name":name, "lastName":lastname, "username":username}, {second like}, {third like}, ..., {nth like}] }, {second post}, {third post}, …, {nth post}] , "error" : [] }</t>
-  </si>
-  <si>
     <t>{userId, timestamp}</t>
   </si>
   <si>
@@ -229,10 +226,10 @@
     <t>post/getComments</t>
   </si>
   <si>
-    <t>{ "data" : [{"postId":id, "text" : text, "url":"url", "timestamp" : timestamp,"userId":id, "name":name, "lastName":lastname, "profilePicture":url, "username":username}, {second comment}, …{nth comment}] , "error" : [] }</t>
-  </si>
-  <si>
-    <t>{ "data" : [postId : {"postId":id, "text" : text, "url":"url", "timestamp" : timestamp,"userId":id, "name":name, "lastName":lastname, "profilePicture":url, "username":username, "comments" : commentsNmbr, "likes": likesNmbr}, secondPost : {secondPost}, .. nthPost : {nthPost}] , "error" : [] }</t>
+    <t>{ "data" : [postId : {"postId":id, "text" : text, "url":"url", "timestamp" : timestamp,"senderId":id, "senderName":name, "senderLastname":lastname, "senderPicture":url, "senderUsername":username, "senderEmail":email,  "recipientId":id, "recipientName":name, "recipientLastname":lastname, "recipientPicture":url, "recipientUsername":username, "recipientEmail":email, "comments" : commentsNmbr, "likes": likesNmbr}, secondPost : {secondPost}, .. nthPost : {nthPost}] , "error" : [] }</t>
+  </si>
+  <si>
+    <t>{ "data" : [{"postId":id, "message" : text, "url":"url", "timestamp" : timestamp,"userId":id, "name":name, "lastName":lastname, "picture":url, "username":username}, {second comment}, …{nth comment}] , "error" : [] }</t>
   </si>
 </sst>
 </file>
@@ -901,9 +898,9 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,7 +964,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -1007,7 +1004,7 @@
         <v>14</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1027,7 +1024,7 @@
         <v>14</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1047,7 +1044,7 @@
         <v>14</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1055,7 +1052,7 @@
         <v>21</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>10</v>
@@ -1067,7 +1064,7 @@
         <v>14</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1087,7 +1084,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1107,7 +1104,7 @@
         <v>14</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1127,7 +1124,7 @@
         <v>14</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1141,13 +1138,13 @@
         <v>10</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1167,7 +1164,7 @@
         <v>14</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1181,38 +1178,38 @@
         <v>10</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>26</v>
@@ -1230,18 +1227,18 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="195" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>14</v>
@@ -1255,7 +1252,7 @@
         <v>38</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>10</v>
@@ -1267,7 +1264,7 @@
         <v>14</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1287,15 +1284,15 @@
         <v>14</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>10</v>
@@ -1307,27 +1304,27 @@
         <v>14</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="C27" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="17" t="s">
+      <c r="E27" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="18" t="s">
         <v>48</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update na newsfeed i wall, dodan getLikes servis
</commit_message>
<xml_diff>
--- a/Dokumenti/DB services.xlsx
+++ b/Dokumenti/DB services.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="61">
   <si>
     <t>SERVISI ZA BAZU</t>
   </si>
@@ -184,9 +184,6 @@
     <t>{userId, postId, flag}</t>
   </si>
   <si>
-    <t>{userId, timestamp}</t>
-  </si>
-  <si>
     <t>post/comment</t>
   </si>
   <si>
@@ -226,10 +223,19 @@
     <t>post/getComments</t>
   </si>
   <si>
-    <t>{ "data" : [postId : {"postId":id, "text" : text, "url":"url", "timestamp" : timestamp,"senderId":id, "senderName":name, "senderLastname":lastname, "senderPicture":url, "senderUsername":username, "senderEmail":email,  "recipientId":id, "recipientName":name, "recipientLastname":lastname, "recipientPicture":url, "recipientUsername":username, "recipientEmail":email, "comments" : commentsNmbr, "likes": likesNmbr}, secondPost : {secondPost}, .. nthPost : {nthPost}] , "error" : [] }</t>
-  </si>
-  <si>
     <t>{ "data" : [{"postId":id, "message" : text, "url":"url", "timestamp" : timestamp,"userId":id, "name":name, "lastName":lastname, "picture":url, "username":username}, {second comment}, …{nth comment}] , "error" : [] }</t>
+  </si>
+  <si>
+    <t>{ "data" : [postId : {"postId":id, "text" : text, "url":"url", "timestamp" : timestamp,"senderId":id, "senderName":name, "senderLastname":lastname, "senderPicture":url, "senderUsername":username, "senderEmail":email,  "recipientId":id, "recipientName":name, "recipientLastname":lastname, "recipientPicture":url, "recipientUsername":username, "recipientEmail":email, "liked": boolean}, secondPost : {secondPost}, .. nthPost : {nthPost}] , "error" : [] }</t>
+  </si>
+  <si>
+    <t>{userId, offset}</t>
+  </si>
+  <si>
+    <t>post/getLikes</t>
+  </si>
+  <si>
+    <t>{ "data" : [{"likeId":id, "timestamp" : timestamp,"userId":id, "name":name, "lastName":lastname, "picture":url, "username":username}, {second comment}, …{nth comment}] , "error" : [] }</t>
   </si>
 </sst>
 </file>
@@ -895,12 +901,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,7 +970,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -1004,7 +1010,7 @@
         <v>14</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1024,7 +1030,7 @@
         <v>14</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1044,7 +1050,7 @@
         <v>14</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1052,7 +1058,7 @@
         <v>21</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>10</v>
@@ -1064,7 +1070,7 @@
         <v>14</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1084,7 +1090,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1104,7 +1110,7 @@
         <v>14</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1124,7 +1130,7 @@
         <v>14</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1138,13 +1144,13 @@
         <v>10</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1164,7 +1170,7 @@
         <v>14</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1178,13 +1184,13 @@
         <v>10</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="180" x14ac:dyDescent="0.25">
@@ -1192,7 +1198,7 @@
         <v>36</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>10</v>
@@ -1204,12 +1210,12 @@
         <v>14</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>26</v>
@@ -1218,13 +1224,13 @@
         <v>10</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="180" x14ac:dyDescent="0.25">
@@ -1232,7 +1238,7 @@
         <v>37</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>10</v>
@@ -1244,7 +1250,7 @@
         <v>14</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1252,7 +1258,7 @@
         <v>38</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>10</v>
@@ -1264,7 +1270,7 @@
         <v>14</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1284,47 +1290,67 @@
         <v>14</v>
       </c>
       <c r="F25" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="15" t="s">
+      <c r="B28" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="C28" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="17" t="s">
+      <c r="E28" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="18" t="s">
         <v>47</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1333,7 +1359,7 @@
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A1:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="F11:F27">
+  <conditionalFormatting sqref="F11:F28">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Active"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Dodani servisi za rad sa galerijom
</commit_message>
<xml_diff>
--- a/Dokumenti/DB services.xlsx
+++ b/Dokumenti/DB services.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="20100" windowHeight="7785"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="63">
   <si>
     <t>SERVISI ZA BAZU</t>
   </si>
@@ -136,15 +136,9 @@
     <t>{postId}</t>
   </si>
   <si>
-    <t>{ userId, imageStream }</t>
-  </si>
-  <si>
     <t>photos/gallery</t>
   </si>
   <si>
-    <t>{ galleryId }</t>
-  </si>
-  <si>
     <t>{ "data" : [ {"postId" : id, "url" : url} , {second Image}, {third Image}, … {nth Image}] , "error" : [] }</t>
   </si>
   <si>
@@ -172,9 +166,6 @@
     <t>post/publish</t>
   </si>
   <si>
-    <t>{ "data" : ["url":url] , "error" : [] }</t>
-  </si>
-  <si>
     <t>{ "data" : ["postId": id] , "error" : [] }</t>
   </si>
   <si>
@@ -239,13 +230,25 @@
   </si>
   <si>
     <t>{ "data" : ["action": "like"/"unlike"] , "error" : [] }</t>
+  </si>
+  <si>
+    <t>user/galleries</t>
+  </si>
+  <si>
+    <t>{ "data" : [ {"albumId" : id, "name" : name} , {second gallery}, {third gallery}, … {nth gallery}] , "error" : [] }</t>
+  </si>
+  <si>
+    <t>{postId, albumId}</t>
+  </si>
+  <si>
+    <t>{albumId}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,7 +324,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -358,6 +361,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14996795556505021"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -522,7 +537,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -563,15 +578,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -594,10 +600,37 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperveza" xfId="1" builtinId="8"/>
-    <cellStyle name="Normalno" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -618,7 +651,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema sustava Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -692,7 +725,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -727,7 +759,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -903,16 +934,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
@@ -921,82 +952,82 @@
     <col min="5" max="5" width="70" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:8" ht="15" customHeight="1">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-    </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-    </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A9" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="19" t="s">
+      <c r="B9" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1" ht="21.75" thickBot="1">
+      <c r="A10" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="30">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -1013,10 +1044,10 @@
         <v>14</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="45">
       <c r="A12" s="11" t="s">
         <v>15</v>
       </c>
@@ -1033,10 +1064,10 @@
         <v>14</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -1053,15 +1084,15 @@
         <v>14</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30">
       <c r="A14" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>10</v>
@@ -1073,287 +1104,307 @@
         <v>14</v>
       </c>
       <c r="F14" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30">
+      <c r="A15" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30">
+      <c r="A16" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30">
+      <c r="A17" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30">
+      <c r="A18" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="60">
+      <c r="A19" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30">
+      <c r="A20" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="90">
+      <c r="A21" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="27" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="8" t="s">
+      <c r="E21" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="180">
+      <c r="A22" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="75">
+      <c r="A23" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="13" t="s">
+      <c r="C23" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="180">
+      <c r="A24" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30">
+      <c r="A25" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30">
+      <c r="A26" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="75">
+      <c r="A27" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30">
+      <c r="A28" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="13" t="s">
+      <c r="B28" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="C28" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="9" t="s">
+      <c r="E28" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="60.75" thickBot="1">
+      <c r="A29" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="B29" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="C29" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="15" t="s">
+      <c r="E29" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="18" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1362,7 +1413,7 @@
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A1:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="F11:F28">
+  <conditionalFormatting sqref="F11:F29">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Active"</formula>
     </cfRule>
@@ -1371,30 +1422,30 @@
     <hyperlink ref="B9" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Popravljeni user/galleries i photos/upload servisi
</commit_message>
<xml_diff>
--- a/Dokumenti/DB services.xlsx
+++ b/Dokumenti/DB services.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="64">
   <si>
     <t>SERVISI ZA BAZU</t>
   </si>
@@ -235,20 +235,48 @@
     <t>user/galleries</t>
   </si>
   <si>
-    <t>{ "data" : [ {"albumId" : id, "name" : name} , {second gallery}, {third gallery}, … {nth gallery}] , "error" : [] }</t>
-  </si>
-  <si>
-    <t>{postId, albumId}</t>
-  </si>
-  <si>
     <t>{albumId}</t>
+  </si>
+  <si>
+    <t>{ "data" : { "url": url } , "error" : [] }</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{userId, url, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OPTIONAL)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> albumId}</t>
+    </r>
+  </si>
+  <si>
+    <t>{ "data" : [ {"albumId" : id, "name" : name, "url" : url} , {second gallery}, {third gallery}, … {nth gallery}] , "error" : [] }</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,6 +351,15 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -591,6 +628,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -599,33 +663,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -938,9 +975,9 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -953,51 +990,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
       <c r="F1" s="18"/>
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1">
       <c r="A9" s="19" t="s">
@@ -1107,120 +1144,120 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30">
-      <c r="A15" s="25" t="s">
+    <row r="15" spans="1:8" ht="45">
+      <c r="A15" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="27" t="s">
+      <c r="C15" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30">
+      <c r="A16" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30">
+      <c r="A17" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30">
+      <c r="A18" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30">
-      <c r="A16" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30">
-      <c r="A17" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="27" t="s">
+      <c r="C18" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="60">
+      <c r="A19" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30">
+      <c r="A20" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30">
-      <c r="A18" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="60">
-      <c r="A19" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30">
-      <c r="A20" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="21" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="10" t="s">
@@ -1228,19 +1265,19 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="90">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="27" t="s">
+      <c r="C21" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E21" s="24" t="s">
         <v>14</v>
       </c>
       <c r="F21" s="14" t="s">
@@ -1248,19 +1285,19 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="180">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="24" t="s">
+      <c r="C22" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="24" t="s">
+      <c r="E22" s="21" t="s">
         <v>14</v>
       </c>
       <c r="F22" s="10" t="s">
@@ -1348,19 +1385,19 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="75">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="27" t="s">
+      <c r="C27" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="24" t="s">
         <v>14</v>
       </c>
       <c r="F27" s="14" t="s">
@@ -1368,19 +1405,19 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="30">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="24" t="s">
+      <c r="C28" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="24" t="s">
+      <c r="E28" s="21" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="10" t="s">
@@ -1388,19 +1425,19 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="60.75" thickBot="1">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="32" t="s">
+      <c r="C29" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="E29" s="32" t="s">
+      <c r="E29" s="29" t="s">
         <v>14</v>
       </c>
       <c r="F29" s="15" t="s">

</xml_diff>

<commit_message>
Search dodan, dodan broj likeova u wall i newsfeed
</commit_message>
<xml_diff>
--- a/Dokumenti/DB services.xlsx
+++ b/Dokumenti/DB services.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="20100" windowHeight="7785"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="63">
   <si>
     <t>SERVISI ZA BAZU</t>
   </si>
@@ -181,12 +181,6 @@
     <t>{userId, query}</t>
   </si>
   <si>
-    <t>{ "data" : [{"userId":id, "name":name, "lastName":lastname, "profilePicture":url, "username":username}, {second user}, {third user}, …,{nth user}] , "error" : [] }</t>
-  </si>
-  <si>
-    <t>Inactive</t>
-  </si>
-  <si>
     <t>Active</t>
   </si>
   <si>
@@ -212,9 +206,6 @@
   </si>
   <si>
     <t>{ "data" : [{"postId":id, "message" : text, "url":"url", "timestamp" : timestamp,"userId":id, "name":name, "lastName":lastname, "picture":url, "username":username}, {second comment}, …{nth comment}] , "error" : [] }</t>
-  </si>
-  <si>
-    <t>{ "data" : [postId : {"postId":id, "text" : text, "url":"url", "timestamp" : timestamp,"senderId":id, "senderName":name, "senderLastname":lastname, "senderPicture":url, "senderUsername":username, "senderEmail":email,  "recipientId":id, "recipientName":name, "recipientLastname":lastname, "recipientPicture":url, "recipientUsername":username, "recipientEmail":email, "liked": boolean}, secondPost : {secondPost}, .. nthPost : {nthPost}] , "error" : [] }</t>
   </si>
   <si>
     <t>{userId, offset}</t>
@@ -271,12 +262,18 @@
   <si>
     <t>{ "data" : [ {"albumId" : id, "name" : name, "url" : url} , {second gallery}, {third gallery}, … {nth gallery}] , "error" : [] }</t>
   </si>
+  <si>
+    <t>{ "data" : [postId : {"postId":id, "text" : text, "url":"url", "timestamp" : timestamp,"senderId":id, "senderName":name, "senderLastname":lastname, "senderPicture":url, "senderUsername":username, "senderEmail":email,  "recipientId":id, "recipientName":name, "recipientLastname":lastname, "recipientPicture":url, "recipientUsername":username, "recipientEmail":email, "liked": boolean, "likesNumber" : number}, secondPost : {secondPost}, .. nthPost : {nthPost}] , "error" : [] }</t>
+  </si>
+  <si>
+    <t>{ "data" : [{"id":id, "name":name, "lastName":lastname, "profilePicture":url, "username":username}, {second user}, {third user}, …,{nth user}] , "error" : [] }</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -666,8 +663,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hiperveza" xfId="1" builtinId="8"/>
+    <cellStyle name="Normalno" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -688,7 +685,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema sustava Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -762,6 +759,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -796,6 +794,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -971,16 +970,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
@@ -989,7 +988,7 @@
     <col min="5" max="5" width="70" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
@@ -1001,7 +1000,7 @@
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32"/>
       <c r="B2" s="32"/>
       <c r="C2" s="32"/>
@@ -1011,7 +1010,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32"/>
       <c r="B3" s="32"/>
       <c r="C3" s="32"/>
@@ -1021,14 +1020,14 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="30"/>
       <c r="C5" s="30"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>2</v>
       </c>
@@ -1036,15 +1035,15 @@
       <c r="C7" s="31"/>
       <c r="D7" s="31"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1">
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" ht="21.75" thickBot="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="16" t="s">
         <v>3</v>
       </c>
@@ -1064,7 +1063,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -1081,10 +1080,10 @@
         <v>14</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>15</v>
       </c>
@@ -1101,10 +1100,10 @@
         <v>14</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -1121,15 +1120,15 @@
         <v>14</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>10</v>
@@ -1141,12 +1140,12 @@
         <v>14</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B15" s="23" t="s">
         <v>16</v>
@@ -1155,16 +1154,16 @@
         <v>10</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E15" s="24" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>23</v>
       </c>
@@ -1181,35 +1180,35 @@
         <v>14</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>25</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C17" s="23" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E17" s="24" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>10</v>
@@ -1221,10 +1220,10 @@
         <v>14</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="60">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>29</v>
       </c>
@@ -1235,16 +1234,16 @@
         <v>10</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E19" s="24" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>31</v>
       </c>
@@ -1261,10 +1260,10 @@
         <v>14</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="90">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>33</v>
       </c>
@@ -1275,38 +1274,38 @@
         <v>10</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E21" s="24" t="s">
         <v>14</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="180">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C22" s="26" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="E22" s="21" t="s">
         <v>14</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="75">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>26</v>
@@ -1315,41 +1314,41 @@
         <v>10</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="180">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="30">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>10</v>
@@ -1361,32 +1360,32 @@
         <v>14</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>38</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E26" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="75">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B27" s="23" t="s">
         <v>26</v>
@@ -1395,21 +1394,21 @@
         <v>10</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E27" s="24" t="s">
         <v>14</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="30">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>39</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C28" s="26" t="s">
         <v>10</v>
@@ -1421,10 +1420,10 @@
         <v>14</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="60.75" thickBot="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="27" t="s">
         <v>40</v>
       </c>
@@ -1435,13 +1434,13 @@
         <v>10</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="E29" s="29" t="s">
         <v>14</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1465,24 +1464,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Dodan servis za dodavanje novog praznog albuma
</commit_message>
<xml_diff>
--- a/Dokumenti/DB services.xlsx
+++ b/Dokumenti/DB services.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="20100" windowHeight="7785"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="73">
   <si>
     <t>SERVISI ZA BAZU</t>
   </si>
@@ -286,12 +286,24 @@
   <si>
     <t>{ "data" : ["statusNumber" : -1/0/1, "status" : none/pending/friends] , "error" : [] }</t>
   </si>
+  <si>
+    <t>user/addGallery</t>
+  </si>
+  <si>
+    <t>{userId, name}</t>
+  </si>
+  <si>
+    <t>{ "data" : { "albumId": id } , "error" : [] }</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -716,6 +728,24 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -725,28 +755,10 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperveza" xfId="1" builtinId="8"/>
-    <cellStyle name="Normalno" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -767,7 +779,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema sustava Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -841,7 +853,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -876,7 +887,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1052,16 +1062,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
@@ -1070,54 +1080,54 @@
     <col min="5" max="5" width="70" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:8" ht="15" customHeight="1">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
       <c r="F1" s="18"/>
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+    <row r="2" spans="1:8" ht="15" customHeight="1">
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
+    <row r="3" spans="1:8" ht="15" customHeight="1">
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+    <row r="5" spans="1:8">
+      <c r="A5" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1">
       <c r="A9" s="19" t="s">
         <v>7</v>
       </c>
@@ -1125,7 +1135,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" s="2" customFormat="1" ht="21.75" thickBot="1">
       <c r="A10" s="16" t="s">
         <v>3</v>
       </c>
@@ -1145,7 +1155,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="30">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -1165,7 +1175,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="45">
       <c r="A12" s="11" t="s">
         <v>15</v>
       </c>
@@ -1185,7 +1195,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="30">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -1205,7 +1215,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="30">
       <c r="A14" s="11" t="s">
         <v>21</v>
       </c>
@@ -1225,7 +1235,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="45">
       <c r="A15" s="22" t="s">
         <v>56</v>
       </c>
@@ -1245,289 +1255,289 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+    <row r="16" spans="1:8" ht="30">
+      <c r="A16" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30">
+      <c r="A17" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B17" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="21" t="s">
+      <c r="C17" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+      <c r="E17" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30">
+      <c r="A18" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B18" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="24" t="s">
+      <c r="C18" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
+      <c r="E18" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30">
+      <c r="A19" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B19" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="21" t="s">
+      <c r="C19" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="E19" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="60">
+      <c r="A20" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B20" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="24" t="s">
+      <c r="C20" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
+      <c r="E20" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30">
+      <c r="A21" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B21" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="21" t="s">
+      <c r="C21" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
+      <c r="E21" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="90">
+      <c r="A22" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B22" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="24" t="s">
+      <c r="C22" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+      <c r="E22" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="180">
+      <c r="A23" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B23" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="21" t="s">
+      <c r="C23" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="E22" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="E23" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="75">
+      <c r="A24" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B24" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="9" t="s">
+      <c r="C24" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="E24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="180">
+      <c r="A25" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B25" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="13" t="s">
+      <c r="C25" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="E25" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30">
+      <c r="A26" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B26" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="9" t="s">
+      <c r="C26" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="E26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="30">
+      <c r="A27" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B27" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="13" t="s">
+      <c r="C27" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
+      <c r="E27" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="75">
+      <c r="A28" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B28" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="24" t="s">
+      <c r="C28" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
+      <c r="E28" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30">
+      <c r="A29" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B29" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="21" t="s">
+      <c r="C29" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="36" t="s">
+      <c r="E29" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30">
+      <c r="A30" s="33" t="s">
         <v>63</v>
-      </c>
-      <c r="B29" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="E29" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="35" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="33" t="s">
-        <v>64</v>
       </c>
       <c r="B30" s="34" t="s">
         <v>30</v>
@@ -1535,39 +1545,39 @@
       <c r="C30" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D30" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="35" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="36" t="s">
+      <c r="E30" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30">
+      <c r="A31" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30">
+      <c r="A32" s="33" t="s">
         <v>65</v>
-      </c>
-      <c r="B31" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="E31" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="35" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="33" t="s">
-        <v>66</v>
       </c>
       <c r="B32" s="34" t="s">
         <v>30</v>
@@ -1575,33 +1585,53 @@
       <c r="C32" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="D32" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30">
+      <c r="A33" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="E32" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="35" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="27" t="s">
+      <c r="E33" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="60.75" thickBot="1">
+      <c r="A34" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B34" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="29" t="s">
+      <c r="C34" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="E33" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="15" t="s">
+      <c r="E34" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="15" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1611,7 +1641,7 @@
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A1:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="F11:F33">
+  <conditionalFormatting sqref="F11:F34">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Active"</formula>
     </cfRule>
@@ -1626,24 +1656,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Promjene za mijenjanje profilne slike, postavljanje aktivnog usera za web, dodan servis user/active (za webase), search promijenjen da za prazan query vraca sve prijatelje korisnika
</commit_message>
<xml_diff>
--- a/Dokumenti/DB services.xlsx
+++ b/Dokumenti/DB services.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="20100" windowHeight="7785"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="75">
   <si>
     <t>SERVISI ZA BAZU</t>
   </si>
@@ -296,14 +296,20 @@
     <t>{ "data" : { "albumId": id } , "error" : [] }</t>
   </si>
   <si>
-    <t>Inactive</t>
+    <t>user/active</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>{ "data" : ["id" : id/-1] , "error" : [] }</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -757,8 +763,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hiperveza" xfId="1" builtinId="8"/>
+    <cellStyle name="Normalno" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -779,7 +785,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema sustava Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -853,6 +859,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -887,6 +894,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1062,16 +1070,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
@@ -1080,7 +1088,7 @@
     <col min="5" max="5" width="70" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
@@ -1092,7 +1100,7 @@
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
       <c r="B2" s="38"/>
       <c r="C2" s="38"/>
@@ -1102,7 +1110,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38"/>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -1112,14 +1120,14 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="36"/>
       <c r="C5" s="36"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
         <v>2</v>
       </c>
@@ -1127,7 +1135,7 @@
       <c r="C7" s="37"/>
       <c r="D7" s="37"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1">
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
         <v>7</v>
       </c>
@@ -1135,7 +1143,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" ht="21.75" thickBot="1">
+    <row r="10" spans="1:8" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="16" t="s">
         <v>3</v>
       </c>
@@ -1155,7 +1163,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -1175,7 +1183,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="45">
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>15</v>
       </c>
@@ -1195,7 +1203,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -1215,7 +1223,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>21</v>
       </c>
@@ -1235,7 +1243,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="45">
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>56</v>
       </c>
@@ -1255,383 +1263,403 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30">
-      <c r="A16" s="22" t="s">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B17" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="24" t="s">
+      <c r="C17" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30">
-      <c r="A17" s="25" t="s">
+      <c r="E17" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B18" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="21" t="s">
+      <c r="C18" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30">
-      <c r="A18" s="22" t="s">
+      <c r="E18" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B19" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="24" t="s">
+      <c r="C19" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30">
-      <c r="A19" s="25" t="s">
+      <c r="E19" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B20" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="21" t="s">
+      <c r="C20" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="60">
-      <c r="A20" s="22" t="s">
+      <c r="E20" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B21" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="24" t="s">
+      <c r="C21" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30">
-      <c r="A21" s="25" t="s">
+      <c r="E21" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B22" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="21" t="s">
+      <c r="C22" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="90">
-      <c r="A22" s="22" t="s">
+      <c r="E22" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B23" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="24" t="s">
+      <c r="C23" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="180">
-      <c r="A23" s="25" t="s">
+      <c r="E23" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B24" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="21" t="s">
+      <c r="C24" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="75">
-      <c r="A24" s="7" t="s">
+      <c r="E24" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B25" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="9" t="s">
+      <c r="C25" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="180">
-      <c r="A25" s="11" t="s">
+      <c r="E25" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B26" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="13" t="s">
+      <c r="C26" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30">
-      <c r="A26" s="7" t="s">
+      <c r="E26" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B27" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="9" t="s">
+      <c r="C27" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="30">
-      <c r="A27" s="11" t="s">
+      <c r="E27" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B28" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="13" t="s">
+      <c r="C28" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="75">
-      <c r="A28" s="22" t="s">
+      <c r="E28" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B29" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="24" t="s">
+      <c r="C29" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="30">
-      <c r="A29" s="25" t="s">
+      <c r="E29" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B30" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="21" t="s">
+      <c r="C30" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="30">
-      <c r="A30" s="33" t="s">
+      <c r="E30" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="34" t="s">
+      <c r="B31" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="35" t="s">
+      <c r="C31" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="30">
-      <c r="A31" s="30" t="s">
+      <c r="E31" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B32" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="21" t="s">
+      <c r="C32" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="E31" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="30">
-      <c r="A32" s="33" t="s">
+      <c r="E32" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="B33" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="35" t="s">
+      <c r="C33" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="E32" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30">
-      <c r="A33" s="30" t="s">
+      <c r="E33" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B34" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="21" t="s">
+      <c r="C34" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="E33" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="60.75" thickBot="1">
-      <c r="A34" s="27" t="s">
+      <c r="E34" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="28" t="s">
+      <c r="B35" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="29" t="s">
+      <c r="C35" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="E34" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="15" t="s">
+      <c r="E35" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="15" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1641,7 +1669,7 @@
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A1:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="F11:F34">
+  <conditionalFormatting sqref="F11:F35">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Active"</formula>
     </cfRule>
@@ -1656,24 +1684,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updejtan upload servis ( sprema sliku i njezin thumbnail na server )
</commit_message>
<xml_diff>
--- a/Dokumenti/DB services.xlsx
+++ b/Dokumenti/DB services.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="20100" windowHeight="7785"/>
@@ -109,12 +109,6 @@
     <t>user/register</t>
   </si>
   <si>
-    <t>{ "data" : ["userId" : id,  "username":username, "name" : name, "lastName" : lastname, "email" : email] , "error" : [] }</t>
-  </si>
-  <si>
-    <t>{username, password, email, name, lastname }</t>
-  </si>
-  <si>
     <t>{ "data" : ["userId" : id] , "error" : [] }</t>
   </si>
   <si>
@@ -193,9 +187,6 @@
     <t>{ "data" : [{"userId": id, "name":name, "lastname":lastname, "lastMessage" : { "message":message, "senderId": sender, "timestamp":timestamp, "flag":flag}}, {second conversation}, {third conversation}, …, {nth conversation}] , "error" : [] }</t>
   </si>
   <si>
-    <t>{username, password, name, lastname }</t>
-  </si>
-  <si>
     <t>{sender, recipient, message, url}</t>
   </si>
   <si>
@@ -205,16 +196,10 @@
     <t>post/getComments</t>
   </si>
   <si>
-    <t>{ "data" : [{"postId":id, "message" : text, "url":"url", "timestamp" : timestamp,"userId":id, "name":name, "lastName":lastname, "picture":url, "username":username}, {second comment}, …{nth comment}] , "error" : [] }</t>
-  </si>
-  <si>
     <t>{userId, offset}</t>
   </si>
   <si>
     <t>post/getLikes</t>
-  </si>
-  <si>
-    <t>{ "data" : [{"likeId":id, "timestamp" : timestamp,"userId":id, "name":name, "lastName":lastname, "picture":url, "username":username}, {second comment}, …{nth comment}] , "error" : [] }</t>
   </si>
   <si>
     <t>{userId, postId}</t>
@@ -266,9 +251,6 @@
     <t>{ "data" : [postId : {"postId":id, "text" : text, "url":"url", "timestamp" : timestamp,"senderId":id, "senderName":name, "senderLastname":lastname, "senderPicture":url, "senderUsername":username, "senderEmail":email,  "recipientId":id, "recipientName":name, "recipientLastname":lastname, "recipientPicture":url, "recipientUsername":username, "recipientEmail":email, "liked": boolean, "likesNumber" : number}, secondPost : {secondPost}, .. nthPost : {nthPost}] , "error" : [] }</t>
   </si>
   <si>
-    <t>{ "data" : [{"id":id, "name":name, "lastName":lastname, "profilePicture":url, "username":username}, {second user}, {third user}, …,{nth user}] , "error" : [] }</t>
-  </si>
-  <si>
     <t>friends/add</t>
   </si>
   <si>
@@ -303,13 +285,31 @@
   </si>
   <si>
     <t>{ "data" : ["id" : id/-1] , "error" : [] }</t>
+  </si>
+  <si>
+    <t>{ "data" : ["username":username, "name" : name, "lastName" : lastname, "picture" : picture, "email" : email] , "error" : [] }</t>
+  </si>
+  <si>
+    <t>{username, password, repeatPassword, email, name, lastname }</t>
+  </si>
+  <si>
+    <t>{username, password, name, lastname, pictureUrl }</t>
+  </si>
+  <si>
+    <t>{ "data" : [{"postId":id, "message" : text, "url":"url", "timestamp" : timestamp,"userId":id, "name":name, "lastName":lastname, "picture":url, "username":username, "email": email}, {second comment}, …{nth comment}] , "error" : [] }</t>
+  </si>
+  <si>
+    <t>{ "data" : [{"likeId":id, "timestamp" : timestamp,"userId":id, "name":name, "lastName":lastname, "picture":url, "username":username, "email": email}, {second comment}, …{nth comment}] , "error" : [] }</t>
+  </si>
+  <si>
+    <t>{ "data" : [{"id":id, "name":name, "lastName":lastname, "picture":url, "username":username}, {second user}, {third user}, …,{nth user}] , "error" : [] }</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -763,8 +763,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperveza" xfId="1" builtinId="8"/>
-    <cellStyle name="Normalno" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -785,7 +785,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema sustava Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -859,7 +859,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -894,7 +893,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1070,25 +1068,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="48.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="70" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
@@ -1100,7 +1098,7 @@
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" customHeight="1">
       <c r="A2" s="38"/>
       <c r="B2" s="38"/>
       <c r="C2" s="38"/>
@@ -1110,7 +1108,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="38"/>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -1120,14 +1118,14 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="36" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="36"/>
       <c r="C5" s="36"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="37" t="s">
         <v>2</v>
       </c>
@@ -1135,15 +1133,15 @@
       <c r="C7" s="37"/>
       <c r="D7" s="37"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="15.75" thickBot="1">
       <c r="A9" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1" ht="21.75" thickBot="1">
       <c r="A10" s="16" t="s">
         <v>3</v>
       </c>
@@ -1163,7 +1161,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="30">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -1180,10 +1178,10 @@
         <v>14</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="45">
       <c r="A12" s="11" t="s">
         <v>15</v>
       </c>
@@ -1194,58 +1192,58 @@
         <v>10</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30">
+      <c r="A14" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="9" t="s">
+      <c r="B14" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>22</v>
-      </c>
       <c r="E14" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="45">
       <c r="A15" s="22" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B15" s="23" t="s">
         <v>16</v>
@@ -1254,158 +1252,158 @@
         <v>10</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E15" s="24" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30">
+      <c r="A16" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30">
+      <c r="A17" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30">
+      <c r="A18" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30">
+      <c r="A19" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30">
+      <c r="A20" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="60">
+      <c r="A21" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="24" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
+      <c r="E21" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30">
+      <c r="A22" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B22" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+      <c r="C22" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="90">
+      <c r="A23" s="22" t="s">
         <v>31</v>
-      </c>
-      <c r="B22" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
-        <v>33</v>
       </c>
       <c r="B23" s="23" t="s">
         <v>16</v>
@@ -1414,253 +1412,253 @@
         <v>10</v>
       </c>
       <c r="D23" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="180">
+      <c r="A24" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="75">
+      <c r="A25" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="180">
+      <c r="A26" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="30">
+      <c r="A27" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30">
+      <c r="A28" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="75">
+      <c r="A29" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30">
+      <c r="A30" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="21" t="s">
+      <c r="C30" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30">
+      <c r="A31" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="13" t="s">
+      <c r="E31" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30">
+      <c r="A32" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+      <c r="E32" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30">
+      <c r="A33" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="30">
+      <c r="A34" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="60.75" thickBot="1">
+      <c r="A35" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="E29" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="25" t="s">
+      <c r="B35" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E30" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="E31" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="E32" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="B33" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="E33" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B35" s="28" t="s">
-        <v>41</v>
-      </c>
       <c r="C35" s="28" t="s">
         <v>10</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="E35" s="29" t="s">
         <v>14</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1684,24 +1682,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Dodan user/requests servis za vraćanje pending friend requestova
</commit_message>
<xml_diff>
--- a/Dokumenti/DB services.xlsx
+++ b/Dokumenti/DB services.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="78">
   <si>
     <t>SERVISI ZA BAZU</t>
   </si>
@@ -303,6 +303,15 @@
   </si>
   <si>
     <t>{ "data" : [{"id":id, "name":name, "lastName":lastname, "picture":url, "username":username}, {second user}, {third user}, …,{nth user}] , "error" : [] }</t>
+  </si>
+  <si>
+    <t>user/requests</t>
+  </si>
+  <si>
+    <t>{ "data" : [ {"id" : id, "name" : name, "lastname" : lastname, "picture" : picture } , {second request}, {third request}, … {nth request}] , "error" : [] }</t>
+  </si>
+  <si>
+    <t>Inactive</t>
   </si>
 </sst>
 </file>
@@ -766,7 +775,14 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1069,12 +1085,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1281,383 +1297,403 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30">
+    <row r="17" spans="1:6" ht="45">
       <c r="A17" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30">
+      <c r="A18" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B18" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="24" t="s">
+      <c r="C18" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30">
-      <c r="A18" s="25" t="s">
+      <c r="E18" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30">
+      <c r="A19" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B19" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="21" t="s">
+      <c r="C19" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30">
-      <c r="A19" s="22" t="s">
+      <c r="E19" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30">
+      <c r="A20" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B20" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="24" t="s">
+      <c r="C20" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30">
-      <c r="A20" s="25" t="s">
+      <c r="E20" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30">
+      <c r="A21" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B21" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="21" t="s">
+      <c r="C21" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="60">
-      <c r="A21" s="22" t="s">
+      <c r="E21" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="60">
+      <c r="A22" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B22" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="24" t="s">
+      <c r="C22" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30">
-      <c r="A22" s="25" t="s">
+      <c r="E22" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30">
+      <c r="A23" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B23" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="21" t="s">
+      <c r="C23" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="90">
-      <c r="A23" s="22" t="s">
+      <c r="E23" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="90">
+      <c r="A24" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B24" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="24" t="s">
+      <c r="C24" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="180">
-      <c r="A24" s="25" t="s">
+      <c r="E24" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="180">
+      <c r="A25" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B25" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="21" t="s">
+      <c r="C25" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="75">
-      <c r="A25" s="7" t="s">
+      <c r="E25" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="75">
+      <c r="A26" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="9" t="s">
+      <c r="C26" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="180">
-      <c r="A26" s="11" t="s">
+      <c r="E26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="180">
+      <c r="A27" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B27" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="13" t="s">
+      <c r="C27" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E26" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="30">
-      <c r="A27" s="7" t="s">
+      <c r="E27" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30">
+      <c r="A28" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B28" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="9" t="s">
+      <c r="C28" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="30">
-      <c r="A28" s="11" t="s">
+      <c r="E28" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30">
+      <c r="A29" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B29" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="13" t="s">
+      <c r="C29" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E28" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="75">
-      <c r="A29" s="22" t="s">
+      <c r="E29" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="75">
+      <c r="A30" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="23" t="s">
+      <c r="B30" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="24" t="s">
+      <c r="C30" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="E29" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="30">
-      <c r="A30" s="25" t="s">
+      <c r="E30" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30">
+      <c r="A31" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B31" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="21" t="s">
+      <c r="C31" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="E30" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="30">
-      <c r="A31" s="33" t="s">
+      <c r="E31" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30">
+      <c r="A32" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="34" t="s">
+      <c r="B32" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="35" t="s">
+      <c r="C32" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="30">
-      <c r="A32" s="30" t="s">
+      <c r="E32" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30">
+      <c r="A33" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B33" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="21" t="s">
+      <c r="C33" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="E32" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30">
-      <c r="A33" s="33" t="s">
+      <c r="E33" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="30">
+      <c r="A34" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="B33" s="34" t="s">
+      <c r="B34" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="35" t="s">
+      <c r="C34" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="E33" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="30">
-      <c r="A34" s="30" t="s">
+      <c r="E34" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="30">
+      <c r="A35" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B35" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="21" t="s">
+      <c r="C35" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="E34" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="60.75" thickBot="1">
-      <c r="A35" s="27" t="s">
+      <c r="E35" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="60.75" thickBot="1">
+      <c r="A36" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="28" t="s">
+      <c r="B36" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="29" t="s">
+      <c r="C36" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="E35" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="15" t="s">
+      <c r="E36" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="15" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1667,8 +1703,8 @@
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A1:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="F11:F35">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="F11:F36">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Active"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Dodan optional userId parametar u photos/gallery servis ( za pregledavanje korisničkih slika u default albumu )
</commit_message>
<xml_diff>
--- a/Dokumenti/DB services.xlsx
+++ b/Dokumenti/DB services.xlsx
@@ -211,9 +211,6 @@
     <t>user/galleries</t>
   </si>
   <si>
-    <t>{albumId}</t>
-  </si>
-  <si>
     <t>{ "data" : { "url": url } , "error" : [] }</t>
   </si>
   <si>
@@ -312,6 +309,34 @@
   </si>
   <si>
     <t>Inactive</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{albumId, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OPTIONAL)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> userId}</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -775,14 +800,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -1088,9 +1106,9 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1208,7 +1226,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>14</v>
@@ -1222,7 +1240,7 @@
         <v>17</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>10</v>
@@ -1242,7 +1260,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>10</v>
@@ -1268,7 +1286,7 @@
         <v>10</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E15" s="24" t="s">
         <v>14</v>
@@ -1279,16 +1297,16 @@
     </row>
     <row r="16" spans="1:8" ht="30">
       <c r="A16" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="C16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="13" t="s">
         <v>67</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>68</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>14</v>
@@ -1299,7 +1317,7 @@
     </row>
     <row r="17" spans="1:6" ht="45">
       <c r="A17" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>16</v>
@@ -1308,27 +1326,27 @@
         <v>10</v>
       </c>
       <c r="D17" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="14" t="s">
         <v>76</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30">
       <c r="A18" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="C18" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="24" t="s">
         <v>64</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>65</v>
       </c>
       <c r="E18" s="24" t="s">
         <v>14</v>
@@ -1362,13 +1380,13 @@
         <v>23</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="23" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E20" s="24" t="s">
         <v>14</v>
@@ -1382,7 +1400,7 @@
         <v>25</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>10</v>
@@ -1468,7 +1486,7 @@
         <v>10</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E25" s="21" t="s">
         <v>14</v>
@@ -1488,7 +1506,7 @@
         <v>10</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>14</v>
@@ -1508,7 +1526,7 @@
         <v>10</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E27" s="13" t="s">
         <v>14</v>
@@ -1568,7 +1586,7 @@
         <v>10</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E30" s="24" t="s">
         <v>14</v>
@@ -1599,7 +1617,7 @@
     </row>
     <row r="32" spans="1:6" ht="30">
       <c r="A32" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" s="34" t="s">
         <v>28</v>
@@ -1608,7 +1626,7 @@
         <v>10</v>
       </c>
       <c r="D32" s="35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E32" s="35" t="s">
         <v>14</v>
@@ -1619,7 +1637,7 @@
     </row>
     <row r="33" spans="1:6" ht="30">
       <c r="A33" s="30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B33" s="31" t="s">
         <v>28</v>
@@ -1628,7 +1646,7 @@
         <v>10</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E33" s="21" t="s">
         <v>14</v>
@@ -1639,7 +1657,7 @@
     </row>
     <row r="34" spans="1:6" ht="30">
       <c r="A34" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B34" s="34" t="s">
         <v>28</v>
@@ -1648,7 +1666,7 @@
         <v>10</v>
       </c>
       <c r="D34" s="35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E34" s="35" t="s">
         <v>14</v>
@@ -1659,7 +1677,7 @@
     </row>
     <row r="35" spans="1:6" ht="30">
       <c r="A35" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B35" s="31" t="s">
         <v>28</v>
@@ -1668,7 +1686,7 @@
         <v>10</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E35" s="21" t="s">
         <v>14</v>
@@ -1688,7 +1706,7 @@
         <v>10</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E36" s="29" t="s">
         <v>14</v>
@@ -1704,7 +1722,7 @@
     <mergeCell ref="A1:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="F11:F36">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Active"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Dodan upload na tudje zidove, konacna dokumentacija
</commit_message>
<xml_diff>
--- a/Dokumenti/DB services.xlsx
+++ b/Dokumenti/DB services.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Ferbook\Projekt\Dokumenti\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="20100" windowHeight="7785"/>
   </bookViews>
@@ -26,7 +21,7 @@
     <author>Vilim Stubičan</author>
   </authors>
   <commentList>
-    <comment ref="D12" authorId="0" shapeId="0">
+    <comment ref="D12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="82">
   <si>
     <t>SERVISI ZA BAZU</t>
   </si>
@@ -217,34 +212,6 @@
   </si>
   <si>
     <t>{ "data" : { "url": url } , "error" : [] }</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">{userId, url, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(OPTIONAL)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> albumId}</t>
-    </r>
   </si>
   <si>
     <t>{ "data" : [ {"albumId" : id, "name" : name, "url" : url} , {second gallery}, {third gallery}, … {nth gallery}] , "error" : [] }</t>
@@ -352,12 +319,65 @@
   <si>
     <t>{ "data" : "base64 encoded image" , "error" : [] }</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{userId, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OPTIONAL)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> userId2, url, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OPTIONAL)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> albumId}</t>
+    </r>
+  </si>
+  <si>
+    <t>{userId, userId2, offset}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,6 +468,14 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -811,17 +839,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperveza" xfId="1" builtinId="8"/>
-    <cellStyle name="Normalno" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -850,7 +871,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema sustava Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -892,7 +913,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -927,7 +948,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1139,9 +1160,9 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1259,7 +1280,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>14</v>
@@ -1273,7 +1294,7 @@
         <v>17</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>10</v>
@@ -1293,7 +1314,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>10</v>
@@ -1319,7 +1340,7 @@
         <v>10</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E15" s="24" t="s">
         <v>14</v>
@@ -1330,16 +1351,16 @@
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="C16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="13" t="s">
         <v>66</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>67</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>14</v>
@@ -1350,7 +1371,7 @@
     </row>
     <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>16</v>
@@ -1359,27 +1380,27 @@
         <v>10</v>
       </c>
       <c r="D17" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="C18" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="24" t="s">
         <v>63</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>64</v>
       </c>
       <c r="E18" s="24" t="s">
         <v>14</v>
@@ -1413,7 +1434,7 @@
         <v>23</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="C20" s="23" t="s">
         <v>10</v>
@@ -1433,7 +1454,7 @@
         <v>25</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>10</v>
@@ -1450,16 +1471,16 @@
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="C22" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="24" t="s">
         <v>79</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>80</v>
       </c>
       <c r="E22" s="24" t="s">
         <v>14</v>
@@ -1539,7 +1560,7 @@
         <v>10</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E26" s="21" t="s">
         <v>14</v>
@@ -1559,7 +1580,7 @@
         <v>10</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>14</v>
@@ -1573,13 +1594,13 @@
         <v>33</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E28" s="13" t="s">
         <v>14</v>
@@ -1639,7 +1660,7 @@
         <v>10</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E31" s="24" t="s">
         <v>14</v>
@@ -1670,7 +1691,7 @@
     </row>
     <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33" s="34" t="s">
         <v>28</v>
@@ -1679,7 +1700,7 @@
         <v>10</v>
       </c>
       <c r="D33" s="35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E33" s="35" t="s">
         <v>14</v>
@@ -1690,7 +1711,7 @@
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B34" s="31" t="s">
         <v>28</v>
@@ -1699,7 +1720,7 @@
         <v>10</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E34" s="21" t="s">
         <v>14</v>
@@ -1710,7 +1731,7 @@
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B35" s="34" t="s">
         <v>28</v>
@@ -1719,7 +1740,7 @@
         <v>10</v>
       </c>
       <c r="D35" s="35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E35" s="35" t="s">
         <v>14</v>
@@ -1730,7 +1751,7 @@
     </row>
     <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B36" s="31" t="s">
         <v>28</v>
@@ -1739,7 +1760,7 @@
         <v>10</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E36" s="21" t="s">
         <v>14</v>
@@ -1759,7 +1780,7 @@
         <v>10</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E37" s="29" t="s">
         <v>14</v>
@@ -1775,12 +1796,12 @@
     <mergeCell ref="A1:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="F11:F21 F23:F37">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Active"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Active"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>